<commit_message>
Bug Fixed & Updates
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\Personal_folder\limchink\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5798BDF0-BCB2-4B6E-9744-43D750C53C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174E7230-3EF9-466D-803A-5B91C6D14647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -396,21 +396,21 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.08984375" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" customWidth="1"/>
-    <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -475,23 +475,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="11.90625" customWidth="1"/>
-    <col min="6" max="6" width="13.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" customWidth="1"/>
-    <col min="11" max="11" width="15.36328125" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -586,17 +586,17 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" customWidth="1"/>
-    <col min="4" max="4" width="14.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,7 +619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Removed is_targsim & Added mca_check.
- Added the recommended user input parameters for different environment instead of adding one extra input parameters.
- Added mca_check user input parameter for mca check method.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\Personal_folder\limchink\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174E7230-3EF9-466D-803A-5B91C6D14647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24BB58-0B29-495C-AB56-823723DF7016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
     <sheet name="aggressive_cont" sheetId="2" r:id="rId2"/>
     <sheet name="aggressive_badname" sheetId="3" r:id="rId3"/>
+    <sheet name="input_guidance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="28">
   <si>
     <t>input_regs</t>
   </si>
@@ -75,14 +76,58 @@
   </si>
   <si>
     <t>auto</t>
+  </si>
+  <si>
+    <t>soc.north.vpupll</t>
+  </si>
+  <si>
+    <t>Running Environment</t>
+  </si>
+  <si>
+    <t>Targsim</t>
+  </si>
+  <si>
+    <t>Post-Si Platform</t>
+  </si>
+  <si>
+    <t>Pre-Si Platform</t>
+  </si>
+  <si>
+    <t>Recommended input</t>
+  </si>
+  <si>
+    <t>TRUE/FALSE</t>
+  </si>
+  <si>
+    <t>mca_check</t>
+  </si>
+  <si>
+    <t>every_failreg</t>
+  </si>
+  <si>
+    <t>every_10val/every_failreg</t>
+  </si>
+  <si>
+    <t>mca_check (it will be ignore if hang_detection is FALSE)</t>
+  </si>
+  <si>
+    <t>every_10val</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -110,9 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,9 +454,10 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,10 +482,13 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -450,16 +500,19 @@
         <v>0</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -472,7 +525,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,6 +542,7 @@
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -517,19 +571,19 @@
         <v>12</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -567,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +637,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -594,6 +648,7 @@
     <col min="4" max="4" width="14.109375" customWidth="1"/>
     <col min="5" max="5" width="16.109375" customWidth="1"/>
     <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -604,19 +659,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -636,13 +691,112 @@
         <v>0</v>
       </c>
       <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEDD8A8-569E-445A-ACF6-90334BB0BE10}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed feedback system from ifelse method to dictionary method and Fixed bugs.
- Now the 2nd failed validation will be able to dump info to fail_log and will not get scripting error anymore.
- Added compare dictionary and use that instead of ifelse function.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\Personal_folder\limchink\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB24BB58-0B29-495C-AB56-823723DF7016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED039800-86AB-4E04-AF14-C25C5500820F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t>auto</t>
   </si>
   <si>
-    <t>soc.north.vpupll</t>
-  </si>
-  <si>
     <t>Running Environment</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>every_10val</t>
+  </si>
+  <si>
+    <t>cdie.atom0.pma_gpsb</t>
   </si>
 </sst>
 </file>
@@ -442,12 +442,12 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.21875" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
@@ -483,12 +483,12 @@
         <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -512,7 +512,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +583,7 @@
         <v>15</v>
       </c>
       <c r="M1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -671,7 +671,7 @@
         <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -721,10 +721,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -741,12 +741,12 @@
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -758,41 +758,41 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated hang output info, Changed attr status & Fixed bug.
- Changed the attributes status from Partial to ToBeTested for easy understanding.
- Added mca hang error code as part of the output.
- Fixed bug for tracking progress bar.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\Personal_folder\limchink\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9279C589-96C8-48BD-B7C9-2DFB429761E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB651F8-A821-419B-9745-CAA35D481589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -156,14 +156,14 @@
     <t>rw/p/l</t>
   </si>
   <si>
-    <t>soc.south.espi.pmc.oob.mem</t>
+    <t>cdie.atom0.pma_gpsb.pma_cr_gpsb_iosfsb_err_status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,14 +180,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -215,12 +207,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +495,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">

</xml_diff>

<commit_message>
Fixed bugs for Pantherlake
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\Personal_folder\limchink\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DB5BB8-6D1C-4C39-A74A-BF61D62A279E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2D0A38-EE02-4E07-8587-F29330C51BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,12 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>input_regs</t>
-  </si>
-  <si>
-    <t>cdie</t>
   </si>
   <si>
     <t>auto_attr</t>
@@ -166,7 +163,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +180,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -210,11 +215,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,69 +520,60 @@
     <col min="9" max="9" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
       <c r="H1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E12" s="3"/>
     </row>
   </sheetData>
@@ -589,7 +586,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,146 +611,152 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -785,30 +788,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -823,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -850,10 +853,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -861,21 +864,21 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -887,46 +890,46 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 'num_val_seq' & 'random' user input to further trim down the validation time.
- It has been tested on ARL-S vpupll ip and it is passed without any error so far.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137526F1-8C98-43BC-8553-4B6B83C3DDC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286FE5FE-74CC-4752-AF08-4BFDEAB7CB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>input_regs</t>
   </si>
@@ -168,7 +168,25 @@
     <t>mca_check (it will be ignore or set to FALSE if hang_detection is FALSE)</t>
   </si>
   <si>
-    <t>soc.pmc.ipc</t>
+    <t>num_val_seq</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>1 or 3</t>
+  </si>
+  <si>
+    <t>we have 3 read-write validation sequences for every single registers. Num_val_seq let user choose how many of this sequence they wanted to run. Only support 1 or 3.</t>
+  </si>
+  <si>
+    <t>soc.north.vpupll</t>
+  </si>
+  <si>
+    <t>FALSE/10/(any number)</t>
+  </si>
+  <si>
+    <t>will randomly choose the registers to validate instead of following the sequence in term of naming. If False, will continue normally. If put any number, AggressiVE will only choose specific number of registers randomly to validate.</t>
   </si>
 </sst>
 </file>
@@ -219,11 +237,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,134 +534,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2" t="s">
+      <c r="J1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="7">
+        <v>3</v>
+      </c>
+      <c r="J2" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
     </row>
   </sheetData>
@@ -648,24 +689,24 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -747,7 +788,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -755,7 +796,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -763,57 +804,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>35</v>
       </c>
@@ -831,18 +872,18 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -865,7 +906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -895,22 +936,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEDD8A8-569E-445A-ACF6-90334BB0BE10}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="65.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -920,7 +963,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -937,88 +980,118 @@
       <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1026,7 +1099,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1034,12 +1107,28 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the user guidance
Contents
- removing aggressive_cont()
- adding 'random' and 'num_val_seq' input parameters
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286FE5FE-74CC-4752-AF08-4BFDEAB7CB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385580A0-DA46-47F3-8574-E27981E66BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,8 +613,8 @@
       <c r="I2" s="7">
         <v>3</v>
       </c>
-      <c r="J2" s="4">
-        <v>10</v>
+      <c r="J2" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added dfd_en input parameter case
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\AggressiVE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DEE2A3-DE73-4299-B3BC-768FB21A3E98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C4D431-9CAA-4152-953C-33EEFE4A9974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>input_regs</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>soc.pmc.mmr</t>
+  </si>
+  <si>
+    <t>dfd_en</t>
   </si>
 </sst>
 </file>
@@ -534,26 +537,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B4:B5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="16.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -584,8 +587,11 @@
       <c r="J1" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
@@ -616,63 +622,66 @@
       <c r="J2" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
     </row>
   </sheetData>
@@ -689,24 +698,24 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -747,7 +756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -788,7 +797,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -796,7 +805,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -804,57 +813,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>35</v>
       </c>
@@ -872,18 +881,18 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -906,7 +915,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -942,18 +951,18 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" customWidth="1"/>
+    <col min="3" max="3" width="16.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="65.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -963,7 +972,7 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -987,7 +996,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1048,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1065,7 +1074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1091,7 +1100,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1107,7 +1116,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1115,7 +1124,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Updated and Added new Features
- make unlockerflush and entercredential as optional when have issue to do so.
- Added post_val for second validation as optional.
- Added Pre_rd_num for user to choose the number of times to do pre_rd (1 or 2)
- Remove compare_in_func() since it's out-to-date and no more using.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C4D431-9CAA-4152-953C-33EEFE4A9974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E820D8E-AE94-4222-9328-A51576271F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14025" yWindow="-12120" windowWidth="19440" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
   <si>
     <t>input_regs</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>dfd_en</t>
+  </si>
+  <si>
+    <t>post_val</t>
+  </si>
+  <si>
+    <t>pre_rd</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -556,7 +562,7 @@
     <col min="9" max="9" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -590,8 +596,14 @@
       <c r="K1" s="4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
@@ -625,48 +637,54 @@
       <c r="K2" s="4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added back aggressive_cont() but in different approach.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E820D8E-AE94-4222-9328-A51576271F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DE5286-EB17-436D-A269-4DD50FC84DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14025" yWindow="-12120" windowWidth="19440" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
   <si>
     <t>input_regs</t>
   </si>
@@ -186,9 +186,6 @@
     <t>will randomly choose the registers to validate instead of following the sequence in term of naming. If False, will continue normally. If put any number, AggressiVE will only choose specific number of registers randomly to validate.</t>
   </si>
   <si>
-    <t>soc.pmc.mmr</t>
-  </si>
-  <si>
     <t>dfd_en</t>
   </si>
   <si>
@@ -196,6 +193,15 @@
   </si>
   <si>
     <t>pre_rd</t>
+  </si>
+  <si>
+    <t>pcd.tam</t>
+  </si>
+  <si>
+    <t>pcd.taps</t>
+  </si>
+  <si>
+    <t>pcd.tcss</t>
   </si>
 </sst>
 </file>
@@ -246,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -255,9 +261,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -545,13 +548,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="35.81640625" customWidth="1"/>
     <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="3" max="3" width="15.26953125" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" customWidth="1"/>
@@ -594,18 +597,18 @@
         <v>47</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
@@ -628,7 +631,7 @@
       <c r="H2" s="4" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>1</v>
       </c>
       <c r="J2" s="4" t="b">
@@ -645,10 +648,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>

</xml_diff>

<commit_message>
Fixed bugs and Removed temporary experiment function.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DE5286-EB17-436D-A269-4DD50FC84DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE8A20-A8EA-4E74-BD49-90BC5526C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
-    <sheet name="aggressive_cont" sheetId="2" r:id="rId2"/>
-    <sheet name="aggressive_badname" sheetId="3" r:id="rId3"/>
-    <sheet name="input_guidance" sheetId="4" r:id="rId4"/>
+    <sheet name="aggressive_badname" sheetId="3" r:id="rId2"/>
+    <sheet name="input_guidance" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>input_regs</t>
   </si>
@@ -48,21 +47,6 @@
     <t>socket</t>
   </si>
   <si>
-    <t>to_exclude</t>
-  </si>
-  <si>
-    <t>pass_regs</t>
-  </si>
-  <si>
-    <t>fail_regs</t>
-  </si>
-  <si>
-    <t>error_regs</t>
-  </si>
-  <si>
-    <t>hang_regs</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -96,57 +80,6 @@
     <t>every_10val</t>
   </si>
   <si>
-    <t>ro/c</t>
-  </si>
-  <si>
-    <t>wo/1</t>
-  </si>
-  <si>
-    <t>wo/c</t>
-  </si>
-  <si>
-    <t>rw/v/p</t>
-  </si>
-  <si>
-    <t>ro/v/p</t>
-  </si>
-  <si>
-    <t>rw/1c/p</t>
-  </si>
-  <si>
-    <t>rw/1s/v</t>
-  </si>
-  <si>
-    <t>rw/o/p</t>
-  </si>
-  <si>
-    <t>rw/o/v/l</t>
-  </si>
-  <si>
-    <t>rw/v2</t>
-  </si>
-  <si>
-    <t>ro/c/v</t>
-  </si>
-  <si>
-    <t>ro/p</t>
-  </si>
-  <si>
-    <t>rw/0c/v</t>
-  </si>
-  <si>
-    <t>rw/p/l</t>
-  </si>
-  <si>
-    <t>soc.south.espi</t>
-  </si>
-  <si>
-    <t>soc.south.spi</t>
-  </si>
-  <si>
-    <t>cdie.atom0</t>
-  </si>
-  <si>
     <t>every_10val/every_failreg/FALSE</t>
   </si>
   <si>
@@ -195,13 +128,13 @@
     <t>pre_rd</t>
   </si>
   <si>
-    <t>pcd.tam</t>
-  </si>
-  <si>
-    <t>pcd.taps</t>
-  </si>
-  <si>
-    <t>pcd.tcss</t>
+    <t>pcd.tcss.tcss_tbt0.cio_vdr_header_00</t>
+  </si>
+  <si>
+    <t>pcd.taps.dfx_pargpcom1.io_muxing_ctrl</t>
+  </si>
+  <si>
+    <t>pcd.tam.iosf_tam_top.i_map_iosf_tam.mode_sel</t>
   </si>
 </sst>
 </file>
@@ -252,9 +185,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -549,7 +481,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,81 +498,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>54</v>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G2" s="4" t="b">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="H2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" s="6">
+      <c r="H2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="4" t="b">
+      <c r="J2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="M2">
@@ -648,68 +580,68 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3"/>
+      <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
+      <c r="A21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -718,189 +650,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D02E66-D43E-4A83-96A4-C72A2BD48F72}">
-  <dimension ref="A1:M15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12.7265625" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="8" max="8" width="13.453125" customWidth="1"/>
-    <col min="9" max="9" width="12.81640625" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD7AC8F6-C58B-41AF-9015-A8D8BB77BE51}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -936,10 +685,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -947,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -962,7 +711,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEDD8A8-569E-445A-ACF6-90334BB0BE10}">
   <dimension ref="A1:H26"/>
   <sheetViews>
@@ -990,149 +739,149 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>47</v>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="4" t="b">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>48</v>
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>48</v>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1140,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1148,23 +897,23 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new feature: aggressive_log()
- This function will rerun all the fields from the desired log file from the desired path.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAE8A20-A8EA-4E74-BD49-90BC5526C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF351FAF-8284-4F80-B00C-41DBF39EBDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="aggressive" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>input_regs</t>
   </si>
@@ -128,13 +128,7 @@
     <t>pre_rd</t>
   </si>
   <si>
-    <t>pcd.tcss.tcss_tbt0.cio_vdr_header_00</t>
-  </si>
-  <si>
-    <t>pcd.taps.dfx_pargpcom1.io_muxing_ctrl</t>
-  </si>
-  <si>
-    <t>pcd.tam.iosf_tam_top.i_map_iosf_tam.mode_sel</t>
+    <t>hub.pcudata.io_boot_fsm_output_override_en1</t>
   </si>
 </sst>
 </file>
@@ -481,23 +475,23 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.81640625" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" customWidth="1"/>
-    <col min="3" max="3" width="15.26953125" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.26953125" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="35.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -538,9 +532,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -564,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" s="3" t="b">
         <v>0</v>
@@ -579,68 +573,64 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>34</v>
-      </c>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>33</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
     </row>
   </sheetData>
@@ -657,18 +647,18 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="6" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,7 +681,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -727,18 +717,18 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="3" max="3" width="16.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="65.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="65.44140625" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -748,7 +738,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -772,7 +762,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -798,7 +788,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -824,7 +814,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -850,7 +840,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -876,7 +866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -884,7 +874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -892,7 +882,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -900,7 +890,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -908,7 +898,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added feature_lock into aggressive_log() and cleaned the code.
Cleaned Area:
- Removed "3"/"1" printed at the end of loading bar.
- Replaced the log files dumping message with the short one and with real path for easy reference.
</commit_message>
<xml_diff>
--- a/input_parameters.xlsx
+++ b/input_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\pgcv04a-cifs.png.intel.com\mve_fvpg_001\IVE_CPV\PM Validation\users\limchink_backup\Github\Aggressive_developer\AggressiVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF351FAF-8284-4F80-B00C-41DBF39EBDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F443BA-D419-40A0-A257-5E0941295503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>input_regs</t>
   </si>
@@ -128,7 +128,10 @@
     <t>pre_rd</t>
   </si>
   <si>
-    <t>hub.pcudata.io_boot_fsm_output_override_en1</t>
+    <t>rw/l</t>
+  </si>
+  <si>
+    <t>hub.ioc_0.iop_vmd_regs.vmconfig_0_14_0_pci</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,10 +537,10 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>

</xml_diff>